<commit_message>
improved territory_options performance (hardcoded via dict comphr)
</commit_message>
<xml_diff>
--- a/pipeline/data_planning/data dictionary - covid.xlsx
+++ b/pipeline/data_planning/data dictionary - covid.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwong/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwong/Programming/Python/DEngineering/covid_de/pipeline/data_planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCE0B43-5445-FE49-AAF7-BCCC94DD1A0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F857ECFB-2BFE-9842-9B7F-B9F6E8E8205C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="640" windowWidth="27640" windowHeight="16440" xr2:uid="{0D3F0011-60C4-3E43-9186-D79D049BCDA3}"/>
+    <workbookView xWindow="1160" yWindow="640" windowWidth="27640" windowHeight="16440" xr2:uid="{0D3F0011-60C4-3E43-9186-D79D049BCDA3}"/>
   </bookViews>
   <sheets>
-    <sheet name="final data tables" sheetId="1" r:id="rId1"/>
+    <sheet name="original data tables - deprecat" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -640,7 +640,7 @@
   <dimension ref="A3:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>